<commit_message>
Fixed error in stated lag time (stated 14 days, should have been 11 days)
</commit_message>
<xml_diff>
--- a/COVID-19_NC_Case_Growth.xlsx
+++ b/COVID-19_NC_Case_Growth.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moglesby/Google Drive/MBO Shared/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moglesby/Google Drive/MBO Shared/COVID-19_NC_Case_Growth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21031259-0826-BA46-B9ED-768A9B258A08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3213A933-F9C2-974B-9DF7-A7712AD0F1BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="480" windowWidth="33600" windowHeight="19240" xr2:uid="{A0B0C22F-6821-2B40-B30A-92DADE45F93A}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="19240" xr2:uid="{A0B0C22F-6821-2B40-B30A-92DADE45F93A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -53,12 +53,6 @@
     <t>Day</t>
   </si>
   <si>
-    <t>NC 7 day lag</t>
-  </si>
-  <si>
-    <t>NC 14 day lag</t>
-  </si>
-  <si>
     <t>NY</t>
   </si>
   <si>
@@ -72,6 +66,9 @@
   </si>
   <si>
     <t>https://www.ncdhhs.gov/covid-19-case-count-nc</t>
+  </si>
+  <si>
+    <t>NC 11 day lag</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +997,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 14 day lag</a:t>
+              <a:t> 11 day lag</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1046,11 +1043,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NC 14 day lag</c:v>
+                  <c:v>NC 11 day lag</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1081,7 +1078,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$17</c:f>
+              <c:f>Sheet1!$F$2:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1138,7 +1135,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$17</c:f>
+              <c:f>Sheet1!$G$2:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1175,7 +1172,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1210,7 +1207,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$17</c:f>
+              <c:f>Sheet1!$F$2:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1267,7 +1264,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$17</c:f>
+              <c:f>Sheet1!$H$2:$H$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1571,7 +1568,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 14 day lag (log scale)</a:t>
+              <a:t> 11 day lag (log scale)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1617,11 +1614,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NC 14 day lag</c:v>
+                  <c:v>NC 11 day lag</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1652,7 +1649,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$17</c:f>
+              <c:f>Sheet1!$F$2:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1709,7 +1706,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$17</c:f>
+              <c:f>Sheet1!$G$2:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1746,7 +1743,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1781,7 +1778,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$17</c:f>
+              <c:f>Sheet1!$F$2:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1838,7 +1835,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$17</c:f>
+              <c:f>Sheet1!$H$2:$H$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -4280,13 +4277,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>6350</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4316,13 +4313,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>184150</xdr:rowOff>
@@ -4354,13 +4351,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>812800</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -4390,13 +4387,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
@@ -4726,15 +4723,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1F3348-3F65-1E4F-A799-445EBB0DDEF9}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+    <sheetView tabSelected="1" topLeftCell="K18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AD30" sqref="AD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4742,516 +4739,461 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43894</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <f>B9</f>
-        <v>7</v>
+      <c r="E2">
+        <v>6</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
         <f>B16</f>
         <v>63</v>
       </c>
-      <c r="I2">
-        <f>F5</f>
+      <c r="H2">
+        <f>E5</f>
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43895</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C14" si="0">B10</f>
-        <v>12</v>
+      <c r="E3">
+        <v>22</v>
       </c>
       <c r="F3">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <f>B17</f>
+        <v>97</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H7" si="1">B17</f>
-        <v>97</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I17" si="2">F6</f>
+        <f t="shared" ref="H3:H17" si="0">E6</f>
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43896</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="E4">
+        <v>33</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <f>B18</f>
+        <v>137</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="F4">
-        <v>33</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="2"/>
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43897</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="D5">
+        <v>341</v>
+      </c>
+      <c r="E5">
+        <v>76</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <f>B19</f>
+        <v>184</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="E5">
-        <v>341</v>
-      </c>
-      <c r="F5">
-        <v>76</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>184</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="2"/>
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43898</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="D6">
+        <v>417</v>
+      </c>
+      <c r="E6">
+        <v>105</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <f>B20</f>
+        <v>255</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="E6">
-        <v>417</v>
-      </c>
-      <c r="F6">
-        <v>105</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>255</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="2"/>
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43899</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="D7">
+        <v>584</v>
+      </c>
+      <c r="E7">
+        <v>142</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <f>B21</f>
+        <v>297</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="E7">
-        <v>584</v>
-      </c>
-      <c r="F7">
-        <v>142</v>
-      </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>297</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="2"/>
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43900</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="D8">
+        <v>778</v>
+      </c>
+      <c r="E8">
+        <v>173</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E8">
-        <v>778</v>
-      </c>
-      <c r="F8">
-        <v>173</v>
-      </c>
-      <c r="G8">
-        <v>7</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="2"/>
         <v>421</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43901</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="D9">
+        <v>1053</v>
+      </c>
+      <c r="E9">
+        <v>216</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="E9">
-        <v>1053</v>
-      </c>
-      <c r="F9">
-        <v>216</v>
-      </c>
-      <c r="G9">
-        <v>8</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="2"/>
         <v>524</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43902</v>
       </c>
       <c r="B10">
         <v>12</v>
       </c>
-      <c r="C10">
+      <c r="D10">
+        <v>1315</v>
+      </c>
+      <c r="E10">
+        <v>216</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="0"/>
-        <v>97</v>
-      </c>
-      <c r="E10">
-        <v>1315</v>
-      </c>
-      <c r="F10">
-        <v>216</v>
-      </c>
-      <c r="G10">
-        <v>9</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="2"/>
         <v>729</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43903</v>
       </c>
       <c r="B11">
         <v>15</v>
       </c>
-      <c r="C11">
+      <c r="D11">
+        <v>1922</v>
+      </c>
+      <c r="E11">
+        <v>421</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="0"/>
-        <v>137</v>
-      </c>
-      <c r="E11">
-        <v>1922</v>
-      </c>
-      <c r="F11">
-        <v>421</v>
-      </c>
-      <c r="G11">
-        <v>10</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="2"/>
         <v>950</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43904</v>
       </c>
       <c r="B12">
         <v>23</v>
       </c>
-      <c r="C12">
+      <c r="D12">
+        <v>1450</v>
+      </c>
+      <c r="E12">
+        <v>524</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="0"/>
-        <v>184</v>
-      </c>
-      <c r="E12">
-        <v>1450</v>
-      </c>
-      <c r="F12">
-        <v>524</v>
-      </c>
-      <c r="G12">
-        <v>11</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="2"/>
         <v>1700</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43905</v>
       </c>
       <c r="B13">
         <v>32</v>
       </c>
-      <c r="C13">
+      <c r="D13">
+        <v>3173</v>
+      </c>
+      <c r="E13">
+        <v>729</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="0"/>
-        <v>255</v>
-      </c>
-      <c r="E13">
-        <v>3173</v>
-      </c>
-      <c r="F13">
-        <v>729</v>
-      </c>
-      <c r="G13">
-        <v>12</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="2"/>
         <v>2382</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43906</v>
       </c>
       <c r="B14">
         <v>33</v>
       </c>
-      <c r="C14">
+      <c r="D14">
+        <v>4019</v>
+      </c>
+      <c r="E14">
+        <v>950</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="0"/>
-        <v>297</v>
-      </c>
-      <c r="E14">
-        <v>4019</v>
-      </c>
-      <c r="F14">
-        <v>950</v>
-      </c>
-      <c r="G14">
-        <v>13</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="2"/>
         <v>4152</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43907</v>
       </c>
       <c r="B15">
         <v>40</v>
       </c>
+      <c r="D15">
+        <v>5723</v>
+      </c>
       <c r="E15">
-        <v>5723</v>
+        <v>1700</v>
       </c>
       <c r="F15">
-        <v>1700</v>
-      </c>
-      <c r="G15">
         <v>14</v>
       </c>
-      <c r="I15">
-        <f t="shared" si="2"/>
+      <c r="H15">
+        <f t="shared" si="0"/>
         <v>7102</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43908</v>
       </c>
       <c r="B16">
         <v>63</v>
       </c>
+      <c r="D16">
+        <v>7731</v>
+      </c>
       <c r="E16">
-        <v>7731</v>
+        <v>2382</v>
       </c>
       <c r="F16">
-        <v>2382</v>
-      </c>
-      <c r="G16">
         <v>15</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="2"/>
+      <c r="H16">
+        <f t="shared" si="0"/>
         <v>10356</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43909</v>
       </c>
       <c r="B17">
         <v>97</v>
       </c>
+      <c r="D17">
+        <v>11723</v>
+      </c>
       <c r="E17">
-        <v>11723</v>
+        <v>4152</v>
       </c>
       <c r="F17">
-        <v>4152</v>
-      </c>
-      <c r="G17">
         <v>16</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="2"/>
+      <c r="H17">
+        <f t="shared" si="0"/>
         <v>15168</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43910</v>
       </c>
       <c r="B18">
         <v>137</v>
       </c>
+      <c r="D18">
+        <v>17038</v>
+      </c>
       <c r="E18">
-        <v>17038</v>
+        <v>7102</v>
       </c>
       <c r="F18">
-        <v>7102</v>
-      </c>
-      <c r="G18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43911</v>
       </c>
       <c r="B19">
         <v>184</v>
       </c>
+      <c r="D19">
+        <v>23203</v>
+      </c>
       <c r="E19">
-        <v>23203</v>
+        <v>10356</v>
       </c>
       <c r="F19">
-        <v>10356</v>
-      </c>
-      <c r="G19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43912</v>
       </c>
       <c r="B20">
         <v>255</v>
       </c>
+      <c r="C20">
+        <v>40</v>
+      </c>
       <c r="D20">
-        <v>40</v>
+        <v>31888</v>
       </c>
       <c r="E20">
-        <v>31888</v>
+        <v>15168</v>
       </c>
       <c r="F20">
-        <v>15168</v>
-      </c>
-      <c r="G20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43913</v>
       </c>
       <c r="B21">
         <v>297</v>
       </c>
-      <c r="D21">
+      <c r="C21">
         <v>46</v>
       </c>
-      <c r="G21">
+      <c r="F21">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>